<commit_message>
Changed the rate of drop item
</commit_message>
<xml_diff>
--- a/Assets/Game/InGame/Enemy/Drop Item/Table/Excel/DropItemTable.xlsx
+++ b/Assets/Game/InGame/Enemy/Drop Item/Table/Excel/DropItemTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vantan\Confront\Assets\Game\InGame\Enemy\Drop Item\Table\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diamo\Desktop\Confront\Confront\Assets\Game\InGame\Enemy\Drop Item\Table\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C153161B-AC76-4843-98ED-C8B02134A552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD22AAC5-9811-4439-A384-6575390E0E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,7 +497,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -660,7 +660,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -775,7 +775,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -802,7 +802,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -958,7 +958,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1114,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D2">
         <v>1</v>

</xml_diff>